<commit_message>
latest stable version with exception and email handling
</commit_message>
<xml_diff>
--- a/Processes/UQGS_EOM_proc_SInetDueDateUpdate_1.0/Data/Config.xlsx
+++ b/Processes/UQGS_EOM_proc_SInetDueDateUpdate_1.0/Data/Config.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="108">
   <si>
     <t>Name</t>
   </si>
@@ -57,9 +57,6 @@
   </si>
   <si>
     <t>ExScreenshotsFolderPath</t>
-  </si>
-  <si>
-    <t>Exceptions_Screenshots</t>
   </si>
   <si>
     <t>Where to save exceptions screenshots - can be a full or a relative path.</t>
@@ -325,6 +322,33 @@
   </si>
   <si>
     <t>mySI-net Home Page URL for DEV environment</t>
+  </si>
+  <si>
+    <t>C:\ExceptionScreenShots\</t>
+  </si>
+  <si>
+    <t>smtpServer</t>
+  </si>
+  <si>
+    <t>smtp.uq.edu.au</t>
+  </si>
+  <si>
+    <t>smtpPort</t>
+  </si>
+  <si>
+    <t>smtp server to use to send emails</t>
+  </si>
+  <si>
+    <t>smtp port number (MUST BE AN INTEGER)</t>
+  </si>
+  <si>
+    <t>c.dudfield@uq.edu.au</t>
+  </si>
+  <si>
+    <t>Email address to send application exception emails to</t>
+  </si>
+  <si>
+    <t>exceptionEmailAddress</t>
   </si>
 </sst>
 </file>
@@ -475,7 +499,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -516,6 +540,13 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="4" builtinId="27"/>
@@ -847,7 +878,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="18.75">
       <c r="A1" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="18.75">
@@ -855,72 +886,72 @@
     </row>
     <row r="3" spans="1:1" ht="60">
       <c r="A3" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.75">
       <c r="A4" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15.75">
       <c r="A6" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="45">
       <c r="A7" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="15.75">
       <c r="A8" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="45">
       <c r="A9" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="45">
       <c r="A10" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="60">
       <c r="A11" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="15.75">
       <c r="A13" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="45">
       <c r="A14" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="15.75">
       <c r="A15" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="30">
       <c r="A16" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:1">
@@ -928,32 +959,32 @@
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="30">
       <c r="A19" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -967,13 +998,13 @@
   <dimension ref="A1:Z993"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="68" customWidth="1"/>
-    <col min="2" max="2" width="104.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="104.28515625" style="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="169.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
@@ -982,7 +1013,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1014,134 +1045,167 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" t="s">
         <v>25</v>
-      </c>
-      <c r="B2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1">
       <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" t="s">
         <v>71</v>
-      </c>
-      <c r="C3" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15" customHeight="1">
       <c r="A4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" t="s">
         <v>73</v>
-      </c>
-      <c r="C4" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15" customHeight="1">
       <c r="A5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B5" t="s">
-        <v>73</v>
+        <v>75</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>72</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15" customHeight="1">
       <c r="A6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B6" t="s">
-        <v>73</v>
+        <v>76</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>72</v>
       </c>
       <c r="C6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1">
       <c r="A7" t="s">
-        <v>78</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>82</v>
+        <v>77</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>81</v>
       </c>
       <c r="C7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15" customHeight="1">
       <c r="A8" t="s">
-        <v>95</v>
-      </c>
-      <c r="B8" s="17" t="s">
         <v>94</v>
       </c>
+      <c r="B8" s="21" t="s">
+        <v>93</v>
+      </c>
       <c r="C8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15" customHeight="1">
       <c r="A9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B9" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="B9" s="17" t="s">
-        <v>97</v>
-      </c>
       <c r="C9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15" customHeight="1">
       <c r="A10" t="s">
-        <v>83</v>
-      </c>
-      <c r="B10" t="s">
-        <v>87</v>
+        <v>82</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>86</v>
       </c>
       <c r="C10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1">
       <c r="A11" t="s">
-        <v>84</v>
-      </c>
-      <c r="B11" t="s">
-        <v>88</v>
+        <v>83</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>87</v>
       </c>
       <c r="C11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15" customHeight="1">
       <c r="A12" t="s">
-        <v>90</v>
-      </c>
-      <c r="B12">
+        <v>89</v>
+      </c>
+      <c r="B12" s="19">
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15" customHeight="1">
       <c r="A13" t="s">
-        <v>91</v>
-      </c>
-      <c r="B13">
+        <v>90</v>
+      </c>
+      <c r="B13" s="19">
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>93</v>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="15" customHeight="1">
+      <c r="A14" t="s">
+        <v>100</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="C14" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="15" customHeight="1">
+      <c r="A15" t="s">
+        <v>102</v>
+      </c>
+      <c r="B15" s="19">
+        <v>587</v>
+      </c>
+      <c r="C15" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="15" customHeight="1">
+      <c r="A16" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="C16" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="21" ht="14.25" customHeight="1"/>
@@ -3179,68 +3243,68 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
         <v>29</v>
-      </c>
-      <c r="C2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" s="3">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -3253,7 +3317,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3306,29 +3370,29 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3">
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
@@ -3336,10 +3400,10 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" t="s">
         <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
@@ -3379,69 +3443,69 @@
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11">
         <v>1000</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12">
         <v>15000</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13">
         <v>60000</v>
       </c>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15">
         <v>0.6</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16">
         <v>0.8</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17">
         <v>0.9</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
@@ -4444,10 +4508,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>

</xml_diff>

<commit_message>
stable working version on the 04072019, still have to test API
</commit_message>
<xml_diff>
--- a/Processes/UQGS_EOM_proc_SInetDueDateUpdate_1.0/Data/Config.xlsx
+++ b/Processes/UQGS_EOM_proc_SInetDueDateUpdate_1.0/Data/Config.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="142">
   <si>
     <t>Name</t>
   </si>
@@ -237,9 +237,6 @@
     <t>Environment</t>
   </si>
   <si>
-    <t>DEV</t>
-  </si>
-  <si>
     <t>Current operating environment. Options are DEV, TEST, STAGING and PROD</t>
   </si>
   <si>
@@ -345,10 +342,115 @@
     <t>c.dudfield@uq.edu.au</t>
   </si>
   <si>
-    <t>Email address to send application exception emails to</t>
-  </si>
-  <si>
-    <t>exceptionEmailAddress</t>
+    <t>mySI_netChecklistManagement_Person_TEST</t>
+  </si>
+  <si>
+    <t>mySI_netChecklistManagement_Person_STAGING</t>
+  </si>
+  <si>
+    <t>mySI_netChecklistManagement_Person_PROD</t>
+  </si>
+  <si>
+    <t>mySI-net Checklist Management Person URL for TEST environment</t>
+  </si>
+  <si>
+    <t>mySI-net Checklist Management Person URL for STAGING environment</t>
+  </si>
+  <si>
+    <t>mySI-net Checklist Management Person URL for PROD environment</t>
+  </si>
+  <si>
+    <t>mySI-net Home Page URL for TEST environment</t>
+  </si>
+  <si>
+    <t>mySI-net Home Page URL for STAGING environment</t>
+  </si>
+  <si>
+    <t>mySI-net Home Page URL for PROD environment</t>
+  </si>
+  <si>
+    <t>mySI_netHomePage_TEST</t>
+  </si>
+  <si>
+    <t>mySI_netHomePage_STAGING</t>
+  </si>
+  <si>
+    <t>mySI_netHomePage_PROD</t>
+  </si>
+  <si>
+    <t>UNITASK_Authorization</t>
+  </si>
+  <si>
+    <t>CIP_Authorization</t>
+  </si>
+  <si>
+    <t>devUNITASK_Authorization</t>
+  </si>
+  <si>
+    <t>Authorization for UniTask API access</t>
+  </si>
+  <si>
+    <t>devCIP_Authorization</t>
+  </si>
+  <si>
+    <t>Authorization for CIP API access</t>
+  </si>
+  <si>
+    <t>API_endPoint_DEV</t>
+  </si>
+  <si>
+    <t>http://localhost:8089/v1/cases/</t>
+  </si>
+  <si>
+    <t>API endpoint to update case status for DEV environment</t>
+  </si>
+  <si>
+    <t>API_endPoint_TEST</t>
+  </si>
+  <si>
+    <t>API_endPoint_STAGING</t>
+  </si>
+  <si>
+    <t>API_endPoint_PROD</t>
+  </si>
+  <si>
+    <t>API endpoint to update case status for TEST environment</t>
+  </si>
+  <si>
+    <t>API endpoint to update case status for STAGING environment</t>
+  </si>
+  <si>
+    <t>API endpoint to update case status for PROD environment</t>
+  </si>
+  <si>
+    <t>exceptionEmailAddress_DEV</t>
+  </si>
+  <si>
+    <t>Email address to send application exception emails to DEV environment</t>
+  </si>
+  <si>
+    <t>Email address to send application exception emails to TEST environment</t>
+  </si>
+  <si>
+    <t>Email address to send application exception emails to STAGING environment</t>
+  </si>
+  <si>
+    <t>Email address to send application exception emails to PROD environment</t>
+  </si>
+  <si>
+    <t>exceptionEmailAddress_TEST</t>
+  </si>
+  <si>
+    <t>exceptionEmailAddress_STAGING</t>
+  </si>
+  <si>
+    <t>exceptionEmailAddress_PROD</t>
+  </si>
+  <si>
+    <t>OperatingEnvironment</t>
+  </si>
+  <si>
+    <t>r.ingram@uq.edu.au</t>
   </si>
 </sst>
 </file>
@@ -995,17 +1097,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z993"/>
+  <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="68" customWidth="1"/>
     <col min="2" max="2" width="104.28515625" style="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="169.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="113.42578125" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1048,7 +1150,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C2" t="s">
         <v>25</v>
@@ -1056,24 +1158,24 @@
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1">
       <c r="A3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>70</v>
+        <v>73</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>71</v>
       </c>
       <c r="C3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15" customHeight="1">
       <c r="A4" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="17" t="s">
-        <v>72</v>
+      <c r="B4" s="19" t="s">
+        <v>71</v>
       </c>
       <c r="C4" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15" customHeight="1">
@@ -1081,7 +1183,7 @@
         <v>75</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C5" t="s">
         <v>78</v>
@@ -1091,8 +1193,8 @@
       <c r="A6" t="s">
         <v>76</v>
       </c>
-      <c r="B6" s="19" t="s">
-        <v>72</v>
+      <c r="B6" s="21" t="s">
+        <v>80</v>
       </c>
       <c r="C6" t="s">
         <v>79</v>
@@ -1100,126 +1202,230 @@
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1">
       <c r="A7" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="C7" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15" customHeight="1">
       <c r="A8" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C8" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15" customHeight="1">
       <c r="A9" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C9" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15" customHeight="1">
       <c r="A10" t="s">
-        <v>82</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>86</v>
+        <v>107</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>92</v>
       </c>
       <c r="C10" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1">
       <c r="A11" t="s">
-        <v>83</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>87</v>
+        <v>94</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>95</v>
       </c>
       <c r="C11" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15" customHeight="1">
       <c r="A12" t="s">
-        <v>89</v>
-      </c>
-      <c r="B12" s="19">
-        <v>6</v>
+        <v>114</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>95</v>
       </c>
       <c r="C12" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15" customHeight="1">
       <c r="A13" t="s">
-        <v>90</v>
-      </c>
-      <c r="B13" s="19">
-        <v>3</v>
+        <v>115</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>95</v>
       </c>
       <c r="C13" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1">
       <c r="A14" t="s">
-        <v>100</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>101</v>
+        <v>116</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>95</v>
       </c>
       <c r="C14" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1">
       <c r="A15" t="s">
+        <v>123</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="C15" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="15" customHeight="1">
+      <c r="A16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="C16" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15" customHeight="1">
+      <c r="A17" t="s">
+        <v>127</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="C17" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15" customHeight="1">
+      <c r="A18" t="s">
+        <v>128</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="C18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15" customHeight="1">
+      <c r="A19" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="C19" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15" customHeight="1">
+      <c r="A20" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="C20" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15" customHeight="1">
+      <c r="A21" s="22" t="s">
+        <v>138</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="C21" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15" customHeight="1">
+      <c r="A22" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="C22" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15" customHeight="1">
+      <c r="A23" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" s="19">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15" customHeight="1">
+      <c r="A24" t="s">
+        <v>89</v>
+      </c>
+      <c r="B24" s="19">
+        <v>3</v>
+      </c>
+      <c r="C24" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15" customHeight="1">
+      <c r="A25" t="s">
+        <v>99</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="C25" t="s">
         <v>102</v>
       </c>
-      <c r="B15" s="19">
+    </row>
+    <row r="26" spans="1:3" ht="15" customHeight="1">
+      <c r="A26" t="s">
+        <v>101</v>
+      </c>
+      <c r="B26" s="19">
         <v>587</v>
       </c>
-      <c r="C15" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="15" customHeight="1">
-      <c r="A16" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="B16" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="C16" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+      <c r="C26" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -2181,6 +2387,12 @@
     <row r="991" ht="14.25" customHeight="1"/>
     <row r="992" ht="14.25" customHeight="1"/>
     <row r="993" ht="14.25" customHeight="1"/>
+    <row r="994" ht="14.25" customHeight="1"/>
+    <row r="995" ht="14.25" customHeight="1"/>
+    <row r="996" ht="14.25" customHeight="1"/>
+    <row r="997" ht="14.25" customHeight="1"/>
+    <row r="998" ht="14.25" customHeight="1"/>
+    <row r="999" ht="14.25" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2192,7 +2404,7 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2236,6 +2448,50 @@
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
+    </row>
+    <row r="2" spans="1:26" ht="15" customHeight="1">
+      <c r="A2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="15" customHeight="1">
+      <c r="A3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="15" customHeight="1">
+      <c r="A4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="15" customHeight="1">
+      <c r="A5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C5" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
@@ -3317,7 +3573,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3400,7 +3656,7 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -4496,11 +4752,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="2" width="65.42578125" customWidth="1"/>
+    <col min="3" max="3" width="71.5703125" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -4537,7 +4797,17 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" t="s">
+        <v>70</v>
+      </c>
+    </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
added asset to config file
</commit_message>
<xml_diff>
--- a/Processes/UQGS_EOM_proc_SInetDueDateUpdate_1.0/Data/Config.xlsx
+++ b/Processes/UQGS_EOM_proc_SInetDueDateUpdate_1.0/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="7" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="145">
   <si>
     <t>Name</t>
   </si>
@@ -237,9 +237,6 @@
     <t>Environment</t>
   </si>
   <si>
-    <t>Current operating environment. Options are DEV, TEST, STAGING and PROD</t>
-  </si>
-  <si>
     <t>https://sa92prep.dev.sinet.uq.edu.au</t>
   </si>
   <si>
@@ -451,6 +448,18 @@
   </si>
   <si>
     <t>r.ingram@uq.edu.au</t>
+  </si>
+  <si>
+    <t>EmailOnSuccess</t>
+  </si>
+  <si>
+    <t>Current operating environment. Options are DEV, TEST, STAGING and PROD (Type: Text)</t>
+  </si>
+  <si>
+    <t>Set this to True to send emails on successful completion (Type: Boolean)</t>
+  </si>
+  <si>
+    <t>EmailOnSuccessFlag</t>
   </si>
 </sst>
 </file>
@@ -1099,8 +1108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1150,7 +1159,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C2" t="s">
         <v>25</v>
@@ -1158,266 +1167,266 @@
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B3" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" t="s">
         <v>71</v>
-      </c>
-      <c r="C3" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15" customHeight="1">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15" customHeight="1">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15" customHeight="1">
       <c r="A6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1">
       <c r="A7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15" customHeight="1">
       <c r="A8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15" customHeight="1">
       <c r="A9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15" customHeight="1">
       <c r="A10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1">
       <c r="A11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="B11" s="21" t="s">
-        <v>95</v>
-      </c>
       <c r="C11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15" customHeight="1">
       <c r="A12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15" customHeight="1">
       <c r="A13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1">
       <c r="A14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1">
       <c r="A15" t="s">
+        <v>122</v>
+      </c>
+      <c r="B15" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="C15" t="s">
         <v>124</v>
-      </c>
-      <c r="C15" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15" customHeight="1">
       <c r="A16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15" customHeight="1">
       <c r="A17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15" customHeight="1">
       <c r="A18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15" customHeight="1">
       <c r="A19" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C19" t="s">
         <v>132</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="C19" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15" customHeight="1">
       <c r="A20" s="22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C20" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15" customHeight="1">
       <c r="A21" s="22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15" customHeight="1">
       <c r="A22" s="22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15" customHeight="1">
       <c r="A23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B23" s="19">
         <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15" customHeight="1">
       <c r="A24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B24" s="19">
         <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15" customHeight="1">
       <c r="A25" t="s">
+        <v>98</v>
+      </c>
+      <c r="B25" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="B25" s="19" t="s">
-        <v>100</v>
-      </c>
       <c r="C25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15" customHeight="1">
       <c r="A26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B26" s="19">
         <v>587</v>
       </c>
       <c r="C26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2404,7 +2413,7 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2451,46 +2460,46 @@
     </row>
     <row r="2" spans="1:26" ht="15" customHeight="1">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1">
       <c r="A3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15" customHeight="1">
       <c r="A4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" t="s">
         <v>119</v>
-      </c>
-      <c r="C4" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15" customHeight="1">
       <c r="A5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" t="s">
         <v>121</v>
-      </c>
-      <c r="C5" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
@@ -3572,8 +3581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3623,7 +3632,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
         <v>44</v>
@@ -3656,7 +3665,7 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -4753,13 +4762,13 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="2" width="65.42578125" customWidth="1"/>
-    <col min="3" max="3" width="71.5703125" customWidth="1"/>
+    <col min="3" max="3" width="88.140625" customWidth="1"/>
     <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4802,13 +4811,23 @@
         <v>69</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C3" t="s">
+        <v>143</v>
+      </c>
+    </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Blackbook commit of working project 05072019
</commit_message>
<xml_diff>
--- a/Processes/UQGS_EOM_proc_SInetDueDateUpdate_1.0/Data/Config.xlsx
+++ b/Processes/UQGS_EOM_proc_SInetDueDateUpdate_1.0/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="7" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="146">
   <si>
     <t>Name</t>
   </si>
@@ -279,15 +279,6 @@
     <t>Orchestrator mySI-net asset credential</t>
   </si>
   <si>
-    <t>CraigADLogin</t>
-  </si>
-  <si>
-    <t>DevSInetLogin</t>
-  </si>
-  <si>
-    <t>testQueue</t>
-  </si>
-  <si>
     <t>partTimeExtension</t>
   </si>
   <si>
@@ -336,9 +327,6 @@
     <t>smtp port number (MUST BE AN INTEGER)</t>
   </si>
   <si>
-    <t>c.dudfield@uq.edu.au</t>
-  </si>
-  <si>
     <t>mySI_netChecklistManagement_Person_TEST</t>
   </si>
   <si>
@@ -381,15 +369,9 @@
     <t>CIP_Authorization</t>
   </si>
   <si>
-    <t>devUNITASK_Authorization</t>
-  </si>
-  <si>
     <t>Authorization for UniTask API access</t>
   </si>
   <si>
-    <t>devCIP_Authorization</t>
-  </si>
-  <si>
     <t>Authorization for CIP API access</t>
   </si>
   <si>
@@ -460,6 +442,27 @@
   </si>
   <si>
     <t>EmailOnSuccessFlag</t>
+  </si>
+  <si>
+    <t>GS_ADLogin1</t>
+  </si>
+  <si>
+    <t>GS_EoM_CIP_Authorization1</t>
+  </si>
+  <si>
+    <t>GS_SInetLogin1</t>
+  </si>
+  <si>
+    <t>EoM-SInet-UpdateDueDate-1.0</t>
+  </si>
+  <si>
+    <t>https://www.sinet.uq.edu.au/psp/ps/EMPLOYEE/SA/c/MANAGE_CHECKLISTS.CHKLST_MANAGEMENT.GBL</t>
+  </si>
+  <si>
+    <t>https://utility.test.api.aws.uq.edu.au/v1/health</t>
+  </si>
+  <si>
+    <t>GS_EoM_UNITASK_Authorization</t>
   </si>
 </sst>
 </file>
@@ -1108,8 +1111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1159,7 +1162,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>86</v>
+        <v>142</v>
       </c>
       <c r="C2" t="s">
         <v>25</v>
@@ -1211,222 +1214,222 @@
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1">
       <c r="A7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" t="s">
         <v>92</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="C7" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15" customHeight="1">
       <c r="A8" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C8" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15" customHeight="1">
       <c r="A9" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C9" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15" customHeight="1">
       <c r="A10" t="s">
-        <v>106</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>91</v>
+        <v>102</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>143</v>
       </c>
       <c r="C10" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1">
       <c r="A11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" t="s">
         <v>93</v>
-      </c>
-      <c r="B11" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="C11" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15" customHeight="1">
       <c r="A12" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C12" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15" customHeight="1">
       <c r="A13" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C13" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1">
       <c r="A14" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C14" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1">
       <c r="A15" t="s">
-        <v>122</v>
-      </c>
-      <c r="B15" s="21" t="s">
-        <v>123</v>
+        <v>116</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>144</v>
       </c>
       <c r="C15" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15" customHeight="1">
       <c r="A16" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C16" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15" customHeight="1">
       <c r="A17" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B17" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="C17" t="s">
         <v>123</v>
-      </c>
-      <c r="C17" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15" customHeight="1">
       <c r="A18" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C18" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15" customHeight="1">
       <c r="A19" s="22" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C19" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15" customHeight="1">
       <c r="A20" s="22" t="s">
-        <v>136</v>
-      </c>
-      <c r="B20" s="21" t="s">
-        <v>103</v>
+        <v>130</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>134</v>
       </c>
       <c r="C20" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15" customHeight="1">
       <c r="A21" s="22" t="s">
-        <v>137</v>
-      </c>
-      <c r="B21" s="21" t="s">
-        <v>103</v>
+        <v>131</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>134</v>
       </c>
       <c r="C21" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15" customHeight="1">
       <c r="A22" s="22" t="s">
-        <v>138</v>
-      </c>
-      <c r="B22" s="21" t="s">
-        <v>103</v>
+        <v>132</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>134</v>
       </c>
       <c r="C22" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15" customHeight="1">
       <c r="A23" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B23" s="19">
         <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15" customHeight="1">
       <c r="A24" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B24" s="19">
         <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15" customHeight="1">
       <c r="A25" t="s">
+        <v>95</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="C25" t="s">
         <v>98</v>
-      </c>
-      <c r="B25" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="C25" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15" customHeight="1">
       <c r="A26" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B26" s="19">
         <v>587</v>
       </c>
       <c r="C26" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2413,7 +2416,7 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2463,7 +2466,7 @@
         <v>80</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>84</v>
+        <v>139</v>
       </c>
       <c r="C2" t="s">
         <v>82</v>
@@ -2474,7 +2477,7 @@
         <v>81</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>85</v>
+        <v>141</v>
       </c>
       <c r="C3" t="s">
         <v>83</v>
@@ -2482,24 +2485,24 @@
     </row>
     <row r="4" spans="1:26" ht="15" customHeight="1">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B4" t="s">
-        <v>118</v>
+        <v>145</v>
       </c>
       <c r="C4" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15" customHeight="1">
       <c r="A5" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B5" t="s">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="C5" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
@@ -3581,8 +3584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3632,7 +3635,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
         <v>44</v>
@@ -3665,7 +3668,7 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -4762,7 +4765,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4811,21 +4814,21 @@
         <v>69</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C2" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B3" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C3" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
API links for test and other environments
</commit_message>
<xml_diff>
--- a/Processes/UQGS_EOM_proc_SInetDueDateUpdate_1.0/Data/Config.xlsx
+++ b/Processes/UQGS_EOM_proc_SInetDueDateUpdate_1.0/Data/Config.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Clients\UQ\DEV\RpaUiPathProcess\Processes\UQGS_EOM_proc_SInetDueDateUpdate_1.0\Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715" activeTab="1"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="23960" windowHeight="16280" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="7" r:id="rId1"/>
@@ -20,11 +15,339 @@
     <sheet name="Assets" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="148">
+  <si>
+    <t>https://business_process.test.api.aws.uq.edu.au/v1/cases</t>
+  </si>
+  <si>
+    <t>https://business_process.stage.api.aws.uq.edu.au/v1/cases</t>
+  </si>
+  <si>
+    <t>https:/business_process.api.uq.edu.au/v1/cases</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Authorization for UniTask API access</t>
+  </si>
+  <si>
+    <t>Authorization for CIP API access</t>
+  </si>
+  <si>
+    <t>API_endPoint_DEV</t>
+  </si>
+  <si>
+    <t>API endpoint to update case status for DEV environment</t>
+  </si>
+  <si>
+    <t>API_endPoint_TEST</t>
+  </si>
+  <si>
+    <t>API_endPoint_STAGING</t>
+  </si>
+  <si>
+    <t>API_endPoint_PROD</t>
+  </si>
+  <si>
+    <t>API endpoint to update case status for TEST environment</t>
+  </si>
+  <si>
+    <t>API endpoint to update case status for STAGING environment</t>
+  </si>
+  <si>
+    <t>API endpoint to update case status for PROD environment</t>
+  </si>
+  <si>
+    <t>exceptionEmailAddress_DEV</t>
+  </si>
+  <si>
+    <t>Email address to send application exception emails to DEV environment</t>
+  </si>
+  <si>
+    <t>Email address to send application exception emails to TEST environment</t>
+  </si>
+  <si>
+    <t>Email address to send application exception emails to STAGING environment</t>
+  </si>
+  <si>
+    <t>Email address to send application exception emails to PROD environment</t>
+  </si>
+  <si>
+    <t>exceptionEmailAddress_TEST</t>
+  </si>
+  <si>
+    <t>exceptionEmailAddress_STAGING</t>
+  </si>
+  <si>
+    <t>exceptionEmailAddress_PROD</t>
+  </si>
+  <si>
+    <t>OperatingEnvironment</t>
+  </si>
+  <si>
+    <t>r.ingram@uq.edu.au</t>
+  </si>
+  <si>
+    <t>EmailOnSuccess</t>
+  </si>
+  <si>
+    <t>Current operating environment. Options are DEV, TEST, STAGING and PROD (Type: Text)</t>
+  </si>
+  <si>
+    <t>Set this to True to send emails on successful completion (Type: Boolean)</t>
+  </si>
+  <si>
+    <t>EmailOnSuccessFlag</t>
+  </si>
+  <si>
+    <t>GS_ADLogin1</t>
+  </si>
+  <si>
+    <t>GS_EoM_CIP_Authorization1</t>
+  </si>
+  <si>
+    <t>GS_SInetLogin1</t>
+  </si>
+  <si>
+    <t>EoM-SInet-UpdateDueDate-1.0</t>
+  </si>
+  <si>
+    <t>https://www.sinet.uq.edu.au/psp/ps/EMPLOYEE/SA/c/MANAGE_CHECKLISTS.CHKLST_MANAGEMENT.GBL</t>
+  </si>
+  <si>
+    <t>GS_EoM_UNITASK_Authorization</t>
+  </si>
+  <si>
+    <t>https://utility.test.api.aws.uq.edu.au/v1/health</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>This key belongs to user designated category 2</t>
+  </si>
+  <si>
+    <t>Task1_Env</t>
+  </si>
+  <si>
+    <t>Task2_Env</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>https://sa92prep.dev.sinet.uq.edu.au</t>
+  </si>
+  <si>
+    <t>mySI-net URL for Dev environment</t>
+  </si>
+  <si>
+    <t>mySI_netURL_DEV</t>
+  </si>
+  <si>
+    <t>mySI_netURL_TEST</t>
+  </si>
+  <si>
+    <t>mySI_netURL_STAGING</t>
+  </si>
+  <si>
+    <t>mySI_netURL_PROD</t>
+  </si>
+  <si>
+    <t>mySI-net URL for Test environment</t>
+  </si>
+  <si>
+    <t>mySI-net URL for Staging environment</t>
+  </si>
+  <si>
+    <t>mySI-net URL for Prod environment</t>
+  </si>
+  <si>
+    <t>https://www.sinet.uq.edu.au/psp/ps/?cmd=login&amp;languageCd=ENG&amp;</t>
+  </si>
+  <si>
+    <t>ADAssetCredential</t>
+  </si>
+  <si>
+    <t>SI_netAssetCredential</t>
+  </si>
+  <si>
+    <t>Orchestrator AD asset credential</t>
+  </si>
+  <si>
+    <t>Orchestrator mySI-net asset credential</t>
+  </si>
+  <si>
+    <t>partTimeExtension</t>
+  </si>
+  <si>
+    <t>fullTimeExtension</t>
+  </si>
+  <si>
+    <t>How many months to extend for part time students (MUST BE AN INTEGER)</t>
+  </si>
+  <si>
+    <t>How many months to extend for full time students (MUST BE AN INTEGER)</t>
+  </si>
+  <si>
+    <t>https://sa92prep.dev.sinet.uq.edu.au/psp/ps/EMPLOYEE/SA/c/MANAGE_CHECKLISTS.CHKLST_MANAGEMENT.GBL</t>
+  </si>
+  <si>
+    <t>mySI_netChecklistManagement_Person_DEV</t>
+  </si>
+  <si>
+    <t>mySI_netHomePage_DEV</t>
+  </si>
+  <si>
+    <t>https://sa92prep.dev.sinet.uq.edu.au/psc/ps/EMPLOYEE/SA/c/NUI_FRAMEWORK.PT_LANDINGPAGE.GBL</t>
+  </si>
+  <si>
+    <t>mySI-net Checklist Management Person URL for DEV environment</t>
+  </si>
+  <si>
+    <t>mySI-net Home Page URL for DEV environment</t>
+  </si>
+  <si>
+    <t>C:\ExceptionScreenShots\</t>
+  </si>
+  <si>
+    <t>smtpServer</t>
+  </si>
+  <si>
+    <t>smtp.uq.edu.au</t>
+  </si>
+  <si>
+    <t>smtpPort</t>
+  </si>
+  <si>
+    <t>smtp server to use to send emails</t>
+  </si>
+  <si>
+    <t>smtp port number (MUST BE AN INTEGER)</t>
+  </si>
+  <si>
+    <t>mySI_netChecklistManagement_Person_TEST</t>
+  </si>
+  <si>
+    <t>mySI_netChecklistManagement_Person_STAGING</t>
+  </si>
+  <si>
+    <t>mySI_netChecklistManagement_Person_PROD</t>
+  </si>
+  <si>
+    <t>mySI-net Checklist Management Person URL for TEST environment</t>
+  </si>
+  <si>
+    <t>mySI-net Checklist Management Person URL for STAGING environment</t>
+  </si>
+  <si>
+    <t>mySI-net Checklist Management Person URL for PROD environment</t>
+  </si>
+  <si>
+    <t>mySI-net Home Page URL for TEST environment</t>
+  </si>
+  <si>
+    <t>mySI-net Home Page URL for STAGING environment</t>
+  </si>
+  <si>
+    <t>mySI-net Home Page URL for PROD environment</t>
+  </si>
+  <si>
+    <t>mySI_netHomePage_TEST</t>
+  </si>
+  <si>
+    <t>mySI_netHomePage_STAGING</t>
+  </si>
+  <si>
+    <t>mySI_netHomePage_PROD</t>
+  </si>
+  <si>
+    <t>UNITASK_Authorization</t>
+  </si>
+  <si>
+    <t>CIP_Authorization</t>
+  </si>
+  <si>
+    <t>FirstRunTask: This task is invoked in the Framework Layer and executes only once(Even if Transaction number 1 were to fail and be retried, it would not be executed again), at program startup. It should not interact with data in memory, since it executes before we enter the main process data layer, but it can be used as a queue dispatcher.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Task1: This task is not invoked anywhere, and should be used by the developer. </t>
+  </si>
+  <si>
+    <t>The sheet contains the list of tasks. Each task is another Business Process Layer context that is executed at some point during the main process execution. For system tasks, the execution is preselected and configurable from the settings. For user added tasks, it is chosen by the user.</t>
+  </si>
+  <si>
+    <t>GetDataTask: This task is invoked in the Data Layer of the main task. The reason is that we might desire it to deliver some TransactionData to us is a safe manner. Thus, it might navigate a website, download a file, process it, and deliver us an output datatable TransactionData. This would be made available in the Data Layer of the main task and would be ready for usage according to the business rules of the process.</t>
+  </si>
+  <si>
+    <t>This sheet is the place to store plain data, as well as most user data with the important exception of credential names.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Typically there is not much for you to add here, although you want to check/change the settings of the Retry mechanism implemented in at the framework layer, during transaction processing, exception recovery, and continuous failiure. Also stores constants used throughout the program, like preconfiguered delays, timeouts. </t>
+  </si>
+  <si>
+    <t>This sheet is used to fetch assets from Orchestrator. The column name is the key, while the column asset hoolds the asset name in Orchestrator. If there is another local key with the same name, it will be overwritten by the value fetched from Orchestrator.</t>
+  </si>
+  <si>
+    <t>####  Legend of Key Value pair colours####</t>
+  </si>
+  <si>
+    <t>Enable the execution of the FirstRun Task. (0=disable, 1=enable)</t>
+  </si>
+  <si>
+    <t>MaxContinuousRetryNumber</t>
+  </si>
+  <si>
+    <t>If &gt; 0 will retry the Initialisation state with a failed exception. Must be an integer.</t>
+  </si>
+  <si>
+    <t>If &gt; 0 will keep a record of consecutive failed exceptions of the Process state. When this number is reached, the application will fail. Must be an integer.</t>
+  </si>
+  <si>
+    <t>If &gt; 0, the robot will retry the same transaction which failed with application exception. This is a local data retry. Orchestrator Queue Item retry are managed at the queue level. Must be integer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You may want to mark keys in this settings dictionary with certain colours. One use I've needed for colors was to define the keys needed in the operation of the framework. </t>
+  </si>
+  <si>
+    <t>This key belongs to user designated category 1</t>
+  </si>
+  <si>
+    <t>This key is used in the Framework layer. You can change the values, but do not delete the keys</t>
+  </si>
+  <si>
+    <t>This key is used in the Business Process Layer. The developer is responsible for the keys. The user is responsible for the values.</t>
+  </si>
+  <si>
+    <t>Help regarding this Configuration File</t>
+  </si>
+  <si>
+    <t>This is the configuration file used to describe various changeable parameters of the process. You should use this file to store settings that are environment related (like paths to programs or resources), user related (email account names, credential names), or plain data (URL of website or name of SAP report to execute). Below, the purpose of each sheet is explained in more detail.</t>
+  </si>
+  <si>
+    <t>Settings</t>
+  </si>
+  <si>
+    <t>Credentials</t>
+  </si>
+  <si>
+    <t>Tasks</t>
+  </si>
+  <si>
+    <t>Constants</t>
+  </si>
+  <si>
+    <t>Assets</t>
+  </si>
+  <si>
+    <t>The credentials sheet is the place to store your credential names.There is also one special credential, that needs to be defined only once, and which is comprised of the URL, TenancyName and CredentialName required to authenticate to the Orchestrator server using REST API. This is only used when working with QueueItems.</t>
+  </si>
   <si>
     <t>Name</t>
   </si>
@@ -148,337 +471,22 @@
   </si>
   <si>
     <t>MaxInitRetryNumber</t>
-  </si>
-  <si>
-    <t>MaxContinuousRetryNumber</t>
-  </si>
-  <si>
-    <t>If &gt; 0 will retry the Initialisation state with a failed exception. Must be an integer.</t>
-  </si>
-  <si>
-    <t>If &gt; 0 will keep a record of consecutive failed exceptions of the Process state. When this number is reached, the application will fail. Must be an integer.</t>
-  </si>
-  <si>
-    <t>If &gt; 0, the robot will retry the same transaction which failed with application exception. This is a local data retry. Orchestrator Queue Item retry are managed at the queue level. Must be integer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You may want to mark keys in this settings dictionary with certain colours. One use I've needed for colors was to define the keys needed in the operation of the framework. </t>
-  </si>
-  <si>
-    <t>This key belongs to user designated category 1</t>
-  </si>
-  <si>
-    <t>This key is used in the Framework layer. You can change the values, but do not delete the keys</t>
-  </si>
-  <si>
-    <t>This key is used in the Business Process Layer. The developer is responsible for the keys. The user is responsible for the values.</t>
-  </si>
-  <si>
-    <t>Help regarding this Configuration File</t>
-  </si>
-  <si>
-    <t>This is the configuration file used to describe various changeable parameters of the process. You should use this file to store settings that are environment related (like paths to programs or resources), user related (email account names, credential names), or plain data (URL of website or name of SAP report to execute). Below, the purpose of each sheet is explained in more detail.</t>
-  </si>
-  <si>
-    <t>Settings</t>
-  </si>
-  <si>
-    <t>Credentials</t>
-  </si>
-  <si>
-    <t>Tasks</t>
-  </si>
-  <si>
-    <t>Constants</t>
-  </si>
-  <si>
-    <t>Assets</t>
-  </si>
-  <si>
-    <t>The credentials sheet is the place to store your credential names.There is also one special credential, that needs to be defined only once, and which is comprised of the URL, TenancyName and CredentialName required to authenticate to the Orchestrator server using REST API. This is only used when working with QueueItems.</t>
-  </si>
-  <si>
-    <t>FirstRunTask: This task is invoked in the Framework Layer and executes only once(Even if Transaction number 1 were to fail and be retried, it would not be executed again), at program startup. It should not interact with data in memory, since it executes before we enter the main process data layer, but it can be used as a queue dispatcher.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Task1: This task is not invoked anywhere, and should be used by the developer. </t>
-  </si>
-  <si>
-    <t>The sheet contains the list of tasks. Each task is another Business Process Layer context that is executed at some point during the main process execution. For system tasks, the execution is preselected and configurable from the settings. For user added tasks, it is chosen by the user.</t>
-  </si>
-  <si>
-    <t>GetDataTask: This task is invoked in the Data Layer of the main task. The reason is that we might desire it to deliver some TransactionData to us is a safe manner. Thus, it might navigate a website, download a file, process it, and deliver us an output datatable TransactionData. This would be made available in the Data Layer of the main task and would be ready for usage according to the business rules of the process.</t>
-  </si>
-  <si>
-    <t>This sheet is the place to store plain data, as well as most user data with the important exception of credential names.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Typically there is not much for you to add here, although you want to check/change the settings of the Retry mechanism implemented in at the framework layer, during transaction processing, exception recovery, and continuous failiure. Also stores constants used throughout the program, like preconfiguered delays, timeouts. </t>
-  </si>
-  <si>
-    <t>This sheet is used to fetch assets from Orchestrator. The column name is the key, while the column asset hoolds the asset name in Orchestrator. If there is another local key with the same name, it will be overwritten by the value fetched from Orchestrator.</t>
-  </si>
-  <si>
-    <t>####  Legend of Key Value pair colours####</t>
-  </si>
-  <si>
-    <t>Enable the execution of the FirstRun Task. (0=disable, 1=enable)</t>
-  </si>
-  <si>
-    <t>This key belongs to user designated category 2</t>
-  </si>
-  <si>
-    <t>Task1_Env</t>
-  </si>
-  <si>
-    <t>Task2_Env</t>
-  </si>
-  <si>
-    <t>Environment</t>
-  </si>
-  <si>
-    <t>https://sa92prep.dev.sinet.uq.edu.au</t>
-  </si>
-  <si>
-    <t>mySI-net URL for Dev environment</t>
-  </si>
-  <si>
-    <t>mySI_netURL_DEV</t>
-  </si>
-  <si>
-    <t>mySI_netURL_TEST</t>
-  </si>
-  <si>
-    <t>mySI_netURL_STAGING</t>
-  </si>
-  <si>
-    <t>mySI_netURL_PROD</t>
-  </si>
-  <si>
-    <t>mySI-net URL for Test environment</t>
-  </si>
-  <si>
-    <t>mySI-net URL for Staging environment</t>
-  </si>
-  <si>
-    <t>mySI-net URL for Prod environment</t>
-  </si>
-  <si>
-    <t>https://www.sinet.uq.edu.au/psp/ps/?cmd=login&amp;languageCd=ENG&amp;</t>
-  </si>
-  <si>
-    <t>ADAssetCredential</t>
-  </si>
-  <si>
-    <t>SI_netAssetCredential</t>
-  </si>
-  <si>
-    <t>Orchestrator AD asset credential</t>
-  </si>
-  <si>
-    <t>Orchestrator mySI-net asset credential</t>
-  </si>
-  <si>
-    <t>partTimeExtension</t>
-  </si>
-  <si>
-    <t>fullTimeExtension</t>
-  </si>
-  <si>
-    <t>How many months to extend for part time students (MUST BE AN INTEGER)</t>
-  </si>
-  <si>
-    <t>How many months to extend for full time students (MUST BE AN INTEGER)</t>
-  </si>
-  <si>
-    <t>https://sa92prep.dev.sinet.uq.edu.au/psp/ps/EMPLOYEE/SA/c/MANAGE_CHECKLISTS.CHKLST_MANAGEMENT.GBL</t>
-  </si>
-  <si>
-    <t>mySI_netChecklistManagement_Person_DEV</t>
-  </si>
-  <si>
-    <t>mySI_netHomePage_DEV</t>
-  </si>
-  <si>
-    <t>https://sa92prep.dev.sinet.uq.edu.au/psc/ps/EMPLOYEE/SA/c/NUI_FRAMEWORK.PT_LANDINGPAGE.GBL</t>
-  </si>
-  <si>
-    <t>mySI-net Checklist Management Person URL for DEV environment</t>
-  </si>
-  <si>
-    <t>mySI-net Home Page URL for DEV environment</t>
-  </si>
-  <si>
-    <t>C:\ExceptionScreenShots\</t>
-  </si>
-  <si>
-    <t>smtpServer</t>
-  </si>
-  <si>
-    <t>smtp.uq.edu.au</t>
-  </si>
-  <si>
-    <t>smtpPort</t>
-  </si>
-  <si>
-    <t>smtp server to use to send emails</t>
-  </si>
-  <si>
-    <t>smtp port number (MUST BE AN INTEGER)</t>
-  </si>
-  <si>
-    <t>mySI_netChecklistManagement_Person_TEST</t>
-  </si>
-  <si>
-    <t>mySI_netChecklistManagement_Person_STAGING</t>
-  </si>
-  <si>
-    <t>mySI_netChecklistManagement_Person_PROD</t>
-  </si>
-  <si>
-    <t>mySI-net Checklist Management Person URL for TEST environment</t>
-  </si>
-  <si>
-    <t>mySI-net Checklist Management Person URL for STAGING environment</t>
-  </si>
-  <si>
-    <t>mySI-net Checklist Management Person URL for PROD environment</t>
-  </si>
-  <si>
-    <t>mySI-net Home Page URL for TEST environment</t>
-  </si>
-  <si>
-    <t>mySI-net Home Page URL for STAGING environment</t>
-  </si>
-  <si>
-    <t>mySI-net Home Page URL for PROD environment</t>
-  </si>
-  <si>
-    <t>mySI_netHomePage_TEST</t>
-  </si>
-  <si>
-    <t>mySI_netHomePage_STAGING</t>
-  </si>
-  <si>
-    <t>mySI_netHomePage_PROD</t>
-  </si>
-  <si>
-    <t>UNITASK_Authorization</t>
-  </si>
-  <si>
-    <t>CIP_Authorization</t>
-  </si>
-  <si>
-    <t>Authorization for UniTask API access</t>
-  </si>
-  <si>
-    <t>Authorization for CIP API access</t>
-  </si>
-  <si>
-    <t>API_endPoint_DEV</t>
-  </si>
-  <si>
-    <t>http://localhost:8089/v1/cases/</t>
-  </si>
-  <si>
-    <t>API endpoint to update case status for DEV environment</t>
-  </si>
-  <si>
-    <t>API_endPoint_TEST</t>
-  </si>
-  <si>
-    <t>API_endPoint_STAGING</t>
-  </si>
-  <si>
-    <t>API_endPoint_PROD</t>
-  </si>
-  <si>
-    <t>API endpoint to update case status for TEST environment</t>
-  </si>
-  <si>
-    <t>API endpoint to update case status for STAGING environment</t>
-  </si>
-  <si>
-    <t>API endpoint to update case status for PROD environment</t>
-  </si>
-  <si>
-    <t>exceptionEmailAddress_DEV</t>
-  </si>
-  <si>
-    <t>Email address to send application exception emails to DEV environment</t>
-  </si>
-  <si>
-    <t>Email address to send application exception emails to TEST environment</t>
-  </si>
-  <si>
-    <t>Email address to send application exception emails to STAGING environment</t>
-  </si>
-  <si>
-    <t>Email address to send application exception emails to PROD environment</t>
-  </si>
-  <si>
-    <t>exceptionEmailAddress_TEST</t>
-  </si>
-  <si>
-    <t>exceptionEmailAddress_STAGING</t>
-  </si>
-  <si>
-    <t>exceptionEmailAddress_PROD</t>
-  </si>
-  <si>
-    <t>OperatingEnvironment</t>
-  </si>
-  <si>
-    <t>r.ingram@uq.edu.au</t>
-  </si>
-  <si>
-    <t>EmailOnSuccess</t>
-  </si>
-  <si>
-    <t>Current operating environment. Options are DEV, TEST, STAGING and PROD (Type: Text)</t>
-  </si>
-  <si>
-    <t>Set this to True to send emails on successful completion (Type: Boolean)</t>
-  </si>
-  <si>
-    <t>EmailOnSuccessFlag</t>
-  </si>
-  <si>
-    <t>GS_ADLogin1</t>
-  </si>
-  <si>
-    <t>GS_EoM_CIP_Authorization1</t>
-  </si>
-  <si>
-    <t>GS_SInetLogin1</t>
-  </si>
-  <si>
-    <t>EoM-SInet-UpdateDueDate-1.0</t>
-  </si>
-  <si>
-    <t>https://www.sinet.uq.edu.au/psp/ps/EMPLOYEE/SA/c/MANAGE_CHECKLISTS.CHKLST_MANAGEMENT.GBL</t>
-  </si>
-  <si>
-    <t>https://utility.test.api.aws.uq.edu.au/v1/health</t>
-  </si>
-  <si>
-    <t>GS_EoM_UNITASK_Authorization</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="12">
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
-      <color rgb="FF000000"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -494,7 +502,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -506,28 +514,26 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
-      <color rgb="FF000000"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
-      <color rgb="FF000000"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -537,6 +543,10 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Verdana"/>
     </font>
   </fonts>
   <fills count="6">
@@ -670,7 +680,7 @@
     <cellStyle name="Note" xfId="3" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -725,7 +735,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -777,7 +787,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -971,101 +981,101 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:A23"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="118" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="18.75">
+    <row r="1" spans="1:1" ht="18">
       <c r="A1" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="18.75">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="18">
       <c r="A2" s="7"/>
     </row>
-    <row r="3" spans="1:1" ht="60">
+    <row r="3" spans="1:1" ht="42">
       <c r="A3" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="15.75">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="15">
       <c r="A4" s="12" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="15.75">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="15">
       <c r="A6" s="12" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" ht="45">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="42">
       <c r="A7" s="13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" ht="15.75">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="15">
       <c r="A8" s="12" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" ht="45">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="28">
       <c r="A9" s="13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" ht="45">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="42">
       <c r="A10" s="13" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" ht="60">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="42">
       <c r="A11" s="13" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="13" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" ht="15.75">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="15">
       <c r="A13" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" ht="45">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="42">
       <c r="A14" s="13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" ht="15.75">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="15">
       <c r="A15" s="12" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" ht="30">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="28">
       <c r="A16" s="13" t="s">
-        <v>63</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:1">
@@ -1073,65 +1083,70 @@
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" ht="30">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="28">
       <c r="A19" s="14" t="s">
-        <v>45</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="9" t="s">
-        <v>47</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="10" t="s">
-        <v>48</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="11" t="s">
-        <v>46</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="15" t="s">
-        <v>66</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="68" customWidth="1"/>
-    <col min="2" max="2" width="104.28515625" style="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="113.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="104.33203125" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="113.5" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>107</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>1</v>
+        <v>108</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>109</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1159,277 +1174,277 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="5" t="s">
-        <v>24</v>
+        <v>131</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>142</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>70</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>71</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15" customHeight="1">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>41</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>70</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>76</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15" customHeight="1">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>42</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>70</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15" customHeight="1">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1">
       <c r="A7" t="s">
-        <v>89</v>
+        <v>57</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>88</v>
+        <v>56</v>
       </c>
       <c r="C7" t="s">
-        <v>92</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15" customHeight="1">
       <c r="A8" t="s">
-        <v>100</v>
+        <v>68</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>88</v>
+        <v>56</v>
       </c>
       <c r="C8" t="s">
-        <v>103</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15" customHeight="1">
       <c r="A9" t="s">
-        <v>101</v>
+        <v>69</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>88</v>
+        <v>56</v>
       </c>
       <c r="C9" t="s">
-        <v>104</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15" customHeight="1">
       <c r="A10" t="s">
-        <v>102</v>
+        <v>70</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>143</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>105</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1">
       <c r="A11" t="s">
-        <v>90</v>
+        <v>58</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>91</v>
+        <v>59</v>
       </c>
       <c r="C11" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15" customHeight="1">
       <c r="A12" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>91</v>
+        <v>59</v>
       </c>
       <c r="C12" t="s">
-        <v>106</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15" customHeight="1">
       <c r="A13" t="s">
-        <v>110</v>
+        <v>78</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>91</v>
+        <v>59</v>
       </c>
       <c r="C13" t="s">
-        <v>107</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1">
       <c r="A14" t="s">
-        <v>111</v>
+        <v>79</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>91</v>
+        <v>59</v>
       </c>
       <c r="C14" t="s">
-        <v>108</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1">
       <c r="A15" t="s">
-        <v>116</v>
+        <v>5</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>144</v>
+        <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>118</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15" customHeight="1">
       <c r="A16" t="s">
-        <v>119</v>
-      </c>
-      <c r="B16" s="21" t="s">
-        <v>117</v>
+        <v>7</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>122</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15" customHeight="1">
       <c r="A17" t="s">
-        <v>120</v>
-      </c>
-      <c r="B17" s="21" t="s">
-        <v>117</v>
+        <v>8</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>123</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15" customHeight="1">
       <c r="A18" t="s">
-        <v>121</v>
+        <v>9</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>117</v>
+        <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>124</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15" customHeight="1">
       <c r="A19" s="22" t="s">
-        <v>125</v>
+        <v>13</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>134</v>
+        <v>22</v>
       </c>
       <c r="C19" t="s">
-        <v>126</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15" customHeight="1">
       <c r="A20" s="22" t="s">
-        <v>130</v>
+        <v>18</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>134</v>
+        <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>127</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15" customHeight="1">
       <c r="A21" s="22" t="s">
-        <v>131</v>
+        <v>19</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>134</v>
+        <v>22</v>
       </c>
       <c r="C21" t="s">
-        <v>128</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15" customHeight="1">
       <c r="A22" s="22" t="s">
-        <v>132</v>
+        <v>20</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>134</v>
+        <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>129</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15" customHeight="1">
       <c r="A23" t="s">
-        <v>84</v>
+        <v>52</v>
       </c>
       <c r="B23" s="19">
         <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15" customHeight="1">
       <c r="A24" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="B24" s="19">
         <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>87</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15" customHeight="1">
       <c r="A25" t="s">
-        <v>95</v>
+        <v>63</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="C25" t="s">
-        <v>98</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15" customHeight="1">
       <c r="A26" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="B26" s="19">
         <v>587</v>
       </c>
       <c r="C26" t="s">
-        <v>99</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2406,36 +2421,41 @@
     <row r="998" ht="14.25" customHeight="1"/>
     <row r="999" ht="14.25" customHeight="1"/>
   </sheetData>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="68" customWidth="1"/>
-    <col min="2" max="2" width="70.140625" customWidth="1"/>
-    <col min="3" max="3" width="169.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="70.1640625" customWidth="1"/>
+    <col min="3" max="3" width="169.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>107</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>108</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>109</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2463,46 +2483,46 @@
     </row>
     <row r="2" spans="1:26" ht="15" customHeight="1">
       <c r="A2" t="s">
-        <v>80</v>
+        <v>48</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>139</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>141</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>83</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15" customHeight="1">
       <c r="A4" t="s">
-        <v>112</v>
+        <v>80</v>
       </c>
       <c r="B4" t="s">
-        <v>145</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>114</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15" customHeight="1">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s">
-        <v>140</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>115</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
@@ -3480,131 +3500,141 @@
     <row r="988" ht="14.25" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="57" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75">
+    <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>107</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>108</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="5" t="s">
-        <v>32</v>
+        <v>139</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>135</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="5" t="s">
-        <v>33</v>
+        <v>140</v>
       </c>
       <c r="B3" s="3">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>65</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="5" t="s">
-        <v>34</v>
+        <v>141</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>143</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="5" t="s">
-        <v>35</v>
+        <v>142</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>37</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="16" t="s">
-        <v>67</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>145</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="16" t="s">
-        <v>68</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>146</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="53" customWidth="1"/>
-    <col min="2" max="2" width="63.5703125" customWidth="1"/>
+    <col min="2" max="2" width="63.5" customWidth="1"/>
     <col min="3" max="3" width="89" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>107</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>108</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>109</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -3632,148 +3662,148 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="5" t="s">
-        <v>3</v>
+        <v>110</v>
       </c>
       <c r="B2" s="2">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>40</v>
+        <v>147</v>
       </c>
       <c r="B3">
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" s="5" t="s">
-        <v>41</v>
+        <v>91</v>
       </c>
       <c r="B4">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" s="5" t="s">
-        <v>10</v>
+        <v>117</v>
       </c>
       <c r="B5" t="s">
-        <v>94</v>
+        <v>62</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>4</v>
+        <v>111</v>
       </c>
       <c r="B7">
         <v>5000</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>6</v>
+        <v>113</v>
       </c>
       <c r="B8">
         <v>30000</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>8</v>
+        <v>115</v>
       </c>
       <c r="B9">
         <v>120000</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" s="4" t="s">
-        <v>12</v>
+        <v>119</v>
       </c>
       <c r="B11">
         <v>1000</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" s="4" t="s">
-        <v>14</v>
+        <v>121</v>
       </c>
       <c r="B12">
         <v>15000</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="4" t="s">
-        <v>16</v>
+        <v>123</v>
       </c>
       <c r="B13">
         <v>60000</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="4" t="s">
-        <v>18</v>
+        <v>125</v>
       </c>
       <c r="B15">
         <v>0.6</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" s="4" t="s">
-        <v>20</v>
+        <v>127</v>
       </c>
       <c r="B16">
         <v>0.8</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" s="4" t="s">
-        <v>22</v>
+        <v>129</v>
       </c>
       <c r="B17">
         <v>0.9</v>
       </c>
       <c r="C17" t="s">
-        <v>23</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
@@ -4757,33 +4787,38 @@
     <row r="998" ht="14.25" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="65.42578125" customWidth="1"/>
-    <col min="3" max="3" width="88.140625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="2" width="65.5" customWidth="1"/>
+    <col min="3" max="3" width="88.1640625" customWidth="1"/>
+    <col min="4" max="26" width="65.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>107</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>133</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>27</v>
+        <v>134</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -4811,24 +4846,24 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>37</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>133</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>136</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>138</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>135</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>137</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -5830,5 +5865,10 @@
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Config file updates for prod - corrected cip api endpoint
</commit_message>
<xml_diff>
--- a/Processes/UQGS_EOM_proc_SInetDueDateUpdate_1.0/Data/Config.xlsx
+++ b/Processes/UQGS_EOM_proc_SInetDueDateUpdate_1.0/Data/Config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="23960" windowHeight="16280" activeTab="1"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="23960" windowHeight="16060" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="7" r:id="rId1"/>
@@ -24,17 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="148">
-  <si>
-    <t>https://business_process.test.api.aws.uq.edu.au/v1/cases</t>
-  </si>
-  <si>
-    <t>https://business_process.stage.api.aws.uq.edu.au/v1/cases</t>
-  </si>
-  <si>
-    <t>https:/business_process.api.uq.edu.au/v1/cases</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="149">
   <si>
     <t>Authorization for UniTask API access</t>
   </si>
@@ -118,9 +108,6 @@
   </si>
   <si>
     <t>EoM-SInet-UpdateDueDate-1.0</t>
-  </si>
-  <si>
-    <t>https://www.sinet.uq.edu.au/psp/ps/EMPLOYEE/SA/c/MANAGE_CHECKLISTS.CHKLST_MANAGEMENT.GBL</t>
   </si>
   <si>
     <t>GS_EoM_UNITASK_Authorization</t>
@@ -169,6 +156,144 @@
     <t>mySI-net URL for Prod environment</t>
   </si>
   <si>
+    <t>https://business_process.api.uq.edu.au/v1/cases</t>
+  </si>
+  <si>
+    <t>Orchestrator mySI-net asset credential</t>
+  </si>
+  <si>
+    <t>partTimeExtension</t>
+  </si>
+  <si>
+    <t>fullTimeExtension</t>
+  </si>
+  <si>
+    <t>How many months to extend for part time students (MUST BE AN INTEGER)</t>
+  </si>
+  <si>
+    <t>How many months to extend for full time students (MUST BE AN INTEGER)</t>
+  </si>
+  <si>
+    <t>https://sa92prep.dev.sinet.uq.edu.au/psp/ps/EMPLOYEE/SA/c/MANAGE_CHECKLISTS.CHKLST_MANAGEMENT.GBL</t>
+  </si>
+  <si>
+    <t>mySI_netChecklistManagement_Person_DEV</t>
+  </si>
+  <si>
+    <t>mySI_netHomePage_DEV</t>
+  </si>
+  <si>
+    <t>https://sa92prep.dev.sinet.uq.edu.au/psc/ps/EMPLOYEE/SA/c/NUI_FRAMEWORK.PT_LANDINGPAGE.GBL</t>
+  </si>
+  <si>
+    <t>mySI-net Checklist Management Person URL for DEV environment</t>
+  </si>
+  <si>
+    <t>mySI-net Home Page URL for DEV environment</t>
+  </si>
+  <si>
+    <t>C:\ExceptionScreenShots\</t>
+  </si>
+  <si>
+    <t>smtpServer</t>
+  </si>
+  <si>
+    <t>smtp.uq.edu.au</t>
+  </si>
+  <si>
+    <t>smtpPort</t>
+  </si>
+  <si>
+    <t>smtp server to use to send emails</t>
+  </si>
+  <si>
+    <t>smtp port number (MUST BE AN INTEGER)</t>
+  </si>
+  <si>
+    <t>mySI_netChecklistManagement_Person_TEST</t>
+  </si>
+  <si>
+    <t>mySI_netChecklistManagement_Person_STAGING</t>
+  </si>
+  <si>
+    <t>mySI_netChecklistManagement_Person_PROD</t>
+  </si>
+  <si>
+    <t>mySI-net Checklist Management Person URL for TEST environment</t>
+  </si>
+  <si>
+    <t>mySI-net Checklist Management Person URL for STAGING environment</t>
+  </si>
+  <si>
+    <t>mySI-net Checklist Management Person URL for PROD environment</t>
+  </si>
+  <si>
+    <t>mySI-net Home Page URL for TEST environment</t>
+  </si>
+  <si>
+    <t>mySI-net Home Page URL for STAGING environment</t>
+  </si>
+  <si>
+    <t>mySI-net Home Page URL for PROD environment</t>
+  </si>
+  <si>
+    <t>mySI_netHomePage_TEST</t>
+  </si>
+  <si>
+    <t>mySI_netHomePage_STAGING</t>
+  </si>
+  <si>
+    <t>mySI_netHomePage_PROD</t>
+  </si>
+  <si>
+    <t>UNITASK_Authorization</t>
+  </si>
+  <si>
+    <t>CIP_Authorization</t>
+  </si>
+  <si>
+    <t>FirstRunTask: This task is invoked in the Framework Layer and executes only once(Even if Transaction number 1 were to fail and be retried, it would not be executed again), at program startup. It should not interact with data in memory, since it executes before we enter the main process data layer, but it can be used as a queue dispatcher.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Task1: This task is not invoked anywhere, and should be used by the developer. </t>
+  </si>
+  <si>
+    <t>https://business_process.test.api.aws.uq.edu.au/v1/cases</t>
+  </si>
+  <si>
+    <t>https://business_process.stage.api.aws.uq.edu.au/v1/cases</t>
+  </si>
+  <si>
+    <t>The sheet contains the list of tasks. Each task is another Business Process Layer context that is executed at some point during the main process execution. For system tasks, the execution is preselected and configurable from the settings. For user added tasks, it is chosen by the user.</t>
+  </si>
+  <si>
+    <t>GetDataTask: This task is invoked in the Data Layer of the main task. The reason is that we might desire it to deliver some TransactionData to us is a safe manner. Thus, it might navigate a website, download a file, process it, and deliver us an output datatable TransactionData. This would be made available in the Data Layer of the main task and would be ready for usage according to the business rules of the process.</t>
+  </si>
+  <si>
+    <t>This sheet is the place to store plain data, as well as most user data with the important exception of credential names.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Typically there is not much for you to add here, although you want to check/change the settings of the Retry mechanism implemented in at the framework layer, during transaction processing, exception recovery, and continuous failiure. Also stores constants used throughout the program, like preconfiguered delays, timeouts. </t>
+  </si>
+  <si>
+    <t>This sheet is used to fetch assets from Orchestrator. The column name is the key, while the column asset hoolds the asset name in Orchestrator. If there is another local key with the same name, it will be overwritten by the value fetched from Orchestrator.</t>
+  </si>
+  <si>
+    <t>####  Legend of Key Value pair colours####</t>
+  </si>
+  <si>
+    <t>Enable the execution of the FirstRun Task. (0=disable, 1=enable)</t>
+  </si>
+  <si>
+    <t>MaxContinuousRetryNumber</t>
+  </si>
+  <si>
+    <t>If &gt; 0 will retry the Initialisation state with a failed exception. Must be an integer.</t>
+  </si>
+  <si>
+    <t>If &gt; 0 will keep a record of consecutive failed exceptions of the Process state. When this number is reached, the application will fail. Must be an integer.</t>
+  </si>
+  <si>
     <t>https://www.sinet.uq.edu.au/psp/ps/?cmd=login&amp;languageCd=ENG&amp;</t>
   </si>
   <si>
@@ -179,138 +304,6 @@
   </si>
   <si>
     <t>Orchestrator AD asset credential</t>
-  </si>
-  <si>
-    <t>Orchestrator mySI-net asset credential</t>
-  </si>
-  <si>
-    <t>partTimeExtension</t>
-  </si>
-  <si>
-    <t>fullTimeExtension</t>
-  </si>
-  <si>
-    <t>How many months to extend for part time students (MUST BE AN INTEGER)</t>
-  </si>
-  <si>
-    <t>How many months to extend for full time students (MUST BE AN INTEGER)</t>
-  </si>
-  <si>
-    <t>https://sa92prep.dev.sinet.uq.edu.au/psp/ps/EMPLOYEE/SA/c/MANAGE_CHECKLISTS.CHKLST_MANAGEMENT.GBL</t>
-  </si>
-  <si>
-    <t>mySI_netChecklistManagement_Person_DEV</t>
-  </si>
-  <si>
-    <t>mySI_netHomePage_DEV</t>
-  </si>
-  <si>
-    <t>https://sa92prep.dev.sinet.uq.edu.au/psc/ps/EMPLOYEE/SA/c/NUI_FRAMEWORK.PT_LANDINGPAGE.GBL</t>
-  </si>
-  <si>
-    <t>mySI-net Checklist Management Person URL for DEV environment</t>
-  </si>
-  <si>
-    <t>mySI-net Home Page URL for DEV environment</t>
-  </si>
-  <si>
-    <t>C:\ExceptionScreenShots\</t>
-  </si>
-  <si>
-    <t>smtpServer</t>
-  </si>
-  <si>
-    <t>smtp.uq.edu.au</t>
-  </si>
-  <si>
-    <t>smtpPort</t>
-  </si>
-  <si>
-    <t>smtp server to use to send emails</t>
-  </si>
-  <si>
-    <t>smtp port number (MUST BE AN INTEGER)</t>
-  </si>
-  <si>
-    <t>mySI_netChecklistManagement_Person_TEST</t>
-  </si>
-  <si>
-    <t>mySI_netChecklistManagement_Person_STAGING</t>
-  </si>
-  <si>
-    <t>mySI_netChecklistManagement_Person_PROD</t>
-  </si>
-  <si>
-    <t>mySI-net Checklist Management Person URL for TEST environment</t>
-  </si>
-  <si>
-    <t>mySI-net Checklist Management Person URL for STAGING environment</t>
-  </si>
-  <si>
-    <t>mySI-net Checklist Management Person URL for PROD environment</t>
-  </si>
-  <si>
-    <t>mySI-net Home Page URL for TEST environment</t>
-  </si>
-  <si>
-    <t>mySI-net Home Page URL for STAGING environment</t>
-  </si>
-  <si>
-    <t>mySI-net Home Page URL for PROD environment</t>
-  </si>
-  <si>
-    <t>mySI_netHomePage_TEST</t>
-  </si>
-  <si>
-    <t>mySI_netHomePage_STAGING</t>
-  </si>
-  <si>
-    <t>mySI_netHomePage_PROD</t>
-  </si>
-  <si>
-    <t>UNITASK_Authorization</t>
-  </si>
-  <si>
-    <t>CIP_Authorization</t>
-  </si>
-  <si>
-    <t>FirstRunTask: This task is invoked in the Framework Layer and executes only once(Even if Transaction number 1 were to fail and be retried, it would not be executed again), at program startup. It should not interact with data in memory, since it executes before we enter the main process data layer, but it can be used as a queue dispatcher.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Task1: This task is not invoked anywhere, and should be used by the developer. </t>
-  </si>
-  <si>
-    <t>The sheet contains the list of tasks. Each task is another Business Process Layer context that is executed at some point during the main process execution. For system tasks, the execution is preselected and configurable from the settings. For user added tasks, it is chosen by the user.</t>
-  </si>
-  <si>
-    <t>GetDataTask: This task is invoked in the Data Layer of the main task. The reason is that we might desire it to deliver some TransactionData to us is a safe manner. Thus, it might navigate a website, download a file, process it, and deliver us an output datatable TransactionData. This would be made available in the Data Layer of the main task and would be ready for usage according to the business rules of the process.</t>
-  </si>
-  <si>
-    <t>This sheet is the place to store plain data, as well as most user data with the important exception of credential names.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Typically there is not much for you to add here, although you want to check/change the settings of the Retry mechanism implemented in at the framework layer, during transaction processing, exception recovery, and continuous failiure. Also stores constants used throughout the program, like preconfiguered delays, timeouts. </t>
-  </si>
-  <si>
-    <t>This sheet is used to fetch assets from Orchestrator. The column name is the key, while the column asset hoolds the asset name in Orchestrator. If there is another local key with the same name, it will be overwritten by the value fetched from Orchestrator.</t>
-  </si>
-  <si>
-    <t>####  Legend of Key Value pair colours####</t>
-  </si>
-  <si>
-    <t>Enable the execution of the FirstRun Task. (0=disable, 1=enable)</t>
-  </si>
-  <si>
-    <t>MaxContinuousRetryNumber</t>
-  </si>
-  <si>
-    <t>If &gt; 0 will retry the Initialisation state with a failed exception. Must be an integer.</t>
-  </si>
-  <si>
-    <t>If &gt; 0 will keep a record of consecutive failed exceptions of the Process state. When this number is reached, the application will fail. Must be an integer.</t>
-  </si>
-  <si>
-    <t>If &gt; 0, the robot will retry the same transaction which failed with application exception. This is a local data retry. Orchestrator Queue Item retry are managed at the queue level. Must be integer</t>
   </si>
   <si>
     <t xml:space="preserve">You may want to mark keys in this settings dictionary with certain colours. One use I've needed for colors was to define the keys needed in the operation of the framework. </t>
@@ -471,6 +464,16 @@
   </si>
   <si>
     <t>MaxInitRetryNumber</t>
+  </si>
+  <si>
+    <t>https://www.sinet.uq.edu.au/psp/ps/EMPLOYEE/SA/c/MANAGE_CHECKLISTS.CHKLST_MANAGEMENT.GBL</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.sinet.uq.edu.au/psc/ps/EMPLOYEE/SA/c/NUI_FRAMEWORK.PT_LANDINGPAGE.GBL</t>
+  </si>
+  <si>
+    <t>If &gt; 0, the robot will retry the same transaction which failed with application exception. This is a local data retry. Orchestrator Queue Item retry are managed at the queue level. Must be integer</t>
   </si>
 </sst>
 </file>
@@ -1002,7 +1005,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="18">
       <c r="A1" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="18">
@@ -1010,72 +1013,72 @@
     </row>
     <row r="3" spans="1:1" ht="42">
       <c r="A3" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15">
       <c r="A4" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="13" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15">
       <c r="A6" s="12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="42">
       <c r="A7" s="13" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="15">
       <c r="A8" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="28">
       <c r="A9" s="13" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="42">
       <c r="A10" s="13" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="42">
       <c r="A11" s="13" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="13" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="15">
       <c r="A13" s="12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="42">
       <c r="A14" s="13" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="15">
       <c r="A15" s="12" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="28">
       <c r="A16" s="13" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:1">
@@ -1083,32 +1086,32 @@
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="8" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="28">
       <c r="A19" s="14" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="15" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1127,7 +1130,7 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -1140,13 +1143,13 @@
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1174,277 +1177,277 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15" customHeight="1">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15" customHeight="1">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15" customHeight="1">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>47</v>
+        <v>89</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C7" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15" customHeight="1">
       <c r="A8" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C8" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15" customHeight="1">
       <c r="A9" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C9" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15" customHeight="1">
       <c r="A10" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>31</v>
+        <v>146</v>
       </c>
       <c r="C10" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C11" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15" customHeight="1">
       <c r="A12" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C12" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15" customHeight="1">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1">
       <c r="A14" t="s">
-        <v>79</v>
-      </c>
-      <c r="B14" s="21" t="s">
-        <v>59</v>
+        <v>72</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>147</v>
       </c>
       <c r="C14" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15" customHeight="1">
       <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" t="s">
         <v>7</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15" customHeight="1">
       <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" t="s">
         <v>8</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15" customHeight="1">
       <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" t="s">
         <v>9</v>
-      </c>
-      <c r="B18" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15" customHeight="1">
       <c r="A19" s="22" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15" customHeight="1">
       <c r="A20" s="22" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15" customHeight="1">
       <c r="A21" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="17" t="s">
-        <v>22</v>
-      </c>
       <c r="C21" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15" customHeight="1">
       <c r="A22" s="22" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C22" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15" customHeight="1">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B23" s="19">
         <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15" customHeight="1">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B24" s="19">
         <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15" customHeight="1">
       <c r="A25" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C25" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15" customHeight="1">
       <c r="A26" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B26" s="19">
         <v>587</v>
       </c>
       <c r="C26" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2449,13 +2452,13 @@
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2483,46 +2486,46 @@
     </row>
     <row r="2" spans="1:26" ht="15" customHeight="1">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>90</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>91</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15" customHeight="1">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15" customHeight="1">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
@@ -3499,6 +3502,7 @@
     <row r="987" ht="14.25" customHeight="1"/>
     <row r="988" ht="14.25" customHeight="1"/>
   </sheetData>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -3525,82 +3529,83 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B3" s="3">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B4" t="s">
         <v>141</v>
       </c>
-      <c r="B4" t="s">
-        <v>143</v>
-      </c>
       <c r="C4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="16" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="16" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -3628,13 +3633,13 @@
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -3662,148 +3667,148 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B2" s="2">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>94</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B3">
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" s="5" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B4">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B7">
         <v>5000</v>
       </c>
       <c r="C7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B8">
         <v>30000</v>
       </c>
       <c r="C8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B9">
         <v>120000</v>
       </c>
       <c r="C9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B11">
         <v>1000</v>
       </c>
       <c r="C11" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B12">
         <v>15000</v>
       </c>
       <c r="C12" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B13">
         <v>60000</v>
       </c>
       <c r="C13" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B15">
         <v>0.6</v>
       </c>
       <c r="C15" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B16">
         <v>0.8</v>
       </c>
       <c r="C16" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B17">
         <v>0.9</v>
       </c>
       <c r="C17" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
@@ -4786,6 +4791,7 @@
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
   </sheetData>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -4812,13 +4818,13 @@
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -4846,24 +4852,24 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B2" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
         <v>21</v>
-      </c>
-      <c r="C2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -5864,6 +5870,7 @@
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">

</xml_diff>

<commit_message>
Commit for fixing ITSADSSD-11963
Ignore checklist rows that do not contain a valid item code
</commit_message>
<xml_diff>
--- a/Processes/UQGS_EOM_proc_SInetDueDateUpdate_1.0/Data/Config.xlsx
+++ b/Processes/UQGS_EOM_proc_SInetDueDateUpdate_1.0/Data/Config.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uqsjose6\workspaces\FORK\RpaUiPathProcess\Processes\UQGS_EOM_proc_SInetDueDateUpdate_1.0\Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="23960" windowHeight="16060" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="23955" windowHeight="16065" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="7" r:id="rId1"/>
@@ -24,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="152">
   <si>
     <t>Authorization for UniTask API access</t>
   </si>
@@ -474,12 +479,21 @@
   </si>
   <si>
     <t>If &gt; 0, the robot will retry the same transaction which failed with application exception. This is a local data retry. Orchestrator Queue Item retry are managed at the queue level. Must be integer</t>
+  </si>
+  <si>
+    <t>List of allowed Item codes</t>
+  </si>
+  <si>
+    <t>CONFIR,EXTCON,MIDREV,EXTMID,THEREV,EXTTHE,SUBMDL,EXTSUB</t>
+  </si>
+  <si>
+    <t>allowedItemList</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="12">
     <font>
       <sz val="11"/>
@@ -984,39 +998,39 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A23"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="118" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="18">
+    <row r="1" spans="1:1" ht="18.75">
       <c r="A1" s="7" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="18">
+    <row r="2" spans="1:1" ht="18.75">
       <c r="A2" s="7"/>
     </row>
-    <row r="3" spans="1:1" ht="42">
+    <row r="3" spans="1:1" ht="60">
       <c r="A3" s="6" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15">
+    <row r="4" spans="1:1" ht="15.75">
       <c r="A4" s="12" t="s">
         <v>99</v>
       </c>
@@ -1026,32 +1040,32 @@
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="15">
+    <row r="6" spans="1:1" ht="15.75">
       <c r="A6" s="12" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="42">
+    <row r="7" spans="1:1" ht="45">
       <c r="A7" s="13" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="15">
+    <row r="8" spans="1:1" ht="15.75">
       <c r="A8" s="12" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="28">
+    <row r="9" spans="1:1" ht="45">
       <c r="A9" s="13" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="42">
+    <row r="10" spans="1:1" ht="45">
       <c r="A10" s="13" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="42">
+    <row r="11" spans="1:1" ht="60">
       <c r="A11" s="13" t="s">
         <v>80</v>
       </c>
@@ -1061,22 +1075,22 @@
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="15">
+    <row r="13" spans="1:1" ht="15.75">
       <c r="A13" s="12" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="42">
+    <row r="14" spans="1:1" ht="45">
       <c r="A14" s="13" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="15">
+    <row r="15" spans="1:1" ht="15.75">
       <c r="A15" s="12" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="28">
+    <row r="16" spans="1:1" ht="30">
       <c r="A16" s="13" t="s">
         <v>83</v>
       </c>
@@ -1089,7 +1103,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="28">
+    <row r="19" spans="1:1" ht="30">
       <c r="A19" s="14" t="s">
         <v>93</v>
       </c>
@@ -1126,19 +1140,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="68" customWidth="1"/>
-    <col min="2" max="2" width="104.33203125" style="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="113.5" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="104.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="113.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1450,7 +1464,17 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A27" t="s">
+        <v>151</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="C27" t="s">
+        <v>149</v>
+      </c>
+    </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2435,19 +2459,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="68" customWidth="1"/>
-    <col min="2" max="2" width="70.1640625" customWidth="1"/>
-    <col min="3" max="3" width="169.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="70.140625" customWidth="1"/>
+    <col min="3" max="3" width="169.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -3513,21 +3537,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="57" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18">
+    <row r="1" spans="1:3" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>105</v>
       </c>
@@ -3616,19 +3640,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="53" customWidth="1"/>
-    <col min="2" max="2" width="63.5" customWidth="1"/>
+    <col min="2" max="2" width="63.42578125" customWidth="1"/>
     <col min="3" max="3" width="89" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -4802,18 +4826,18 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="65.5" customWidth="1"/>
-    <col min="3" max="3" width="88.1640625" customWidth="1"/>
-    <col min="4" max="26" width="65.5" customWidth="1"/>
+    <col min="1" max="2" width="65.42578125" customWidth="1"/>
+    <col min="3" max="3" width="88.140625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Modified files for enhancement ITSADSSD-11963
Ignore checklist rows that do not contain a valid item code
</commit_message>
<xml_diff>
--- a/Processes/UQGS_EOM_proc_SInetDueDateUpdate_1.0/Data/Config.xlsx
+++ b/Processes/UQGS_EOM_proc_SInetDueDateUpdate_1.0/Data/Config.xlsx
@@ -481,13 +481,13 @@
     <t>If &gt; 0, the robot will retry the same transaction which failed with application exception. This is a local data retry. Orchestrator Queue Item retry are managed at the queue level. Must be integer</t>
   </si>
   <si>
+    <t>allowedItemList</t>
+  </si>
+  <si>
+    <t>CONFIR,EXTCON,MIDREV,EXTMID,THEREV,EXTTHE,SUBMDL,EXTSUB</t>
+  </si>
+  <si>
     <t>List of allowed Item codes</t>
-  </si>
-  <si>
-    <t>CONFIR,EXTCON,MIDREV,EXTMID,THEREV,EXTTHE,SUBMDL,EXTSUB</t>
-  </si>
-  <si>
-    <t>allowedItemList</t>
   </si>
 </sst>
 </file>
@@ -1144,7 +1144,7 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="A27" sqref="A27:C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1466,13 +1466,13 @@
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B27" s="19" t="s">
         <v>150</v>
       </c>
       <c r="C27" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
ITSADSSD-11963 - Removed delays and added Delay between keys
</commit_message>
<xml_diff>
--- a/Processes/UQGS_EOM_proc_SInetDueDateUpdate_1.0/Data/Config.xlsx
+++ b/Processes/UQGS_EOM_proc_SInetDueDateUpdate_1.0/Data/Config.xlsx
@@ -88,9 +88,6 @@
     <t>OperatingEnvironment</t>
   </si>
   <si>
-    <t>r.ingram@uq.edu.au</t>
-  </si>
-  <si>
     <t>EmailOnSuccess</t>
   </si>
   <si>
@@ -488,6 +485,9 @@
   </si>
   <si>
     <t>List of allowed Item codes</t>
+  </si>
+  <si>
+    <t>bpm.ads@its.uq.edu.au</t>
   </si>
 </sst>
 </file>
@@ -1019,7 +1019,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="18.75">
       <c r="A1" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="18.75">
@@ -1027,72 +1027,72 @@
     </row>
     <row r="3" spans="1:1" ht="60">
       <c r="A3" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.75">
       <c r="A4" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15.75">
       <c r="A6" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="45">
       <c r="A7" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="15.75">
       <c r="A8" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="45">
       <c r="A9" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="45">
       <c r="A10" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="60">
       <c r="A11" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="15.75">
       <c r="A13" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="45">
       <c r="A14" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="15.75">
       <c r="A15" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="30">
       <c r="A16" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:1">
@@ -1100,32 +1100,32 @@
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="30">
       <c r="A19" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1143,9 +1143,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:C27"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -1157,13 +1155,13 @@
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="C1" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1191,145 +1189,145 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
         <v>129</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
         <v>34</v>
-      </c>
-      <c r="C3" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15" customHeight="1">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15" customHeight="1">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15" customHeight="1">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15" customHeight="1">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15" customHeight="1">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15" customHeight="1">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1">
       <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="21" t="s">
-        <v>52</v>
-      </c>
       <c r="C11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15" customHeight="1">
       <c r="A12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15" customHeight="1">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1">
       <c r="A14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1">
@@ -1337,7 +1335,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C15" t="s">
         <v>3</v>
@@ -1348,7 +1346,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>
@@ -1359,7 +1357,7 @@
         <v>5</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
@@ -1370,7 +1368,7 @@
         <v>6</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C18" t="s">
         <v>9</v>
@@ -1381,7 +1379,7 @@
         <v>10</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>19</v>
+        <v>151</v>
       </c>
       <c r="C19" t="s">
         <v>11</v>
@@ -1392,7 +1390,7 @@
         <v>15</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>19</v>
+        <v>151</v>
       </c>
       <c r="C20" t="s">
         <v>12</v>
@@ -1403,7 +1401,7 @@
         <v>16</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>19</v>
+        <v>151</v>
       </c>
       <c r="C21" t="s">
         <v>13</v>
@@ -1414,7 +1412,7 @@
         <v>17</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>19</v>
+        <v>151</v>
       </c>
       <c r="C22" t="s">
         <v>14</v>
@@ -1422,57 +1420,57 @@
     </row>
     <row r="23" spans="1:3" ht="15" customHeight="1">
       <c r="A23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B23" s="19">
         <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15" customHeight="1">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B24" s="19">
         <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15" customHeight="1">
       <c r="A25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="B25" s="19" t="s">
-        <v>57</v>
-      </c>
       <c r="C25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15" customHeight="1">
       <c r="A26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B26" s="19">
         <v>587</v>
       </c>
       <c r="C26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" t="s">
+        <v>148</v>
+      </c>
+      <c r="B27" s="19" t="s">
         <v>149</v>
       </c>
-      <c r="B27" s="19" t="s">
+      <c r="C27" t="s">
         <v>150</v>
-      </c>
-      <c r="C27" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2476,13 +2474,13 @@
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2510,32 +2508,32 @@
     </row>
     <row r="2" spans="1:26" ht="15" customHeight="1">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15" customHeight="1">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
@@ -2543,10 +2541,10 @@
     </row>
     <row r="5" spans="1:26" ht="15" customHeight="1">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
@@ -3553,79 +3551,79 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18.75">
       <c r="A1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C2" t="s">
         <v>133</v>
-      </c>
-      <c r="C2" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B3" s="3">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -3657,13 +3655,13 @@
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -3691,148 +3689,148 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B2" s="2">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B3">
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B4">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" t="s">
         <v>115</v>
-      </c>
-      <c r="B5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B7">
         <v>5000</v>
       </c>
       <c r="C7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B8">
         <v>30000</v>
       </c>
       <c r="C8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B9">
         <v>120000</v>
       </c>
       <c r="C9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B11">
         <v>1000</v>
       </c>
       <c r="C11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B12">
         <v>15000</v>
       </c>
       <c r="C12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B13">
         <v>60000</v>
       </c>
       <c r="C13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B15">
         <v>0.6</v>
       </c>
       <c r="C15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B16">
         <v>0.8</v>
       </c>
       <c r="C16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B17">
         <v>0.9</v>
       </c>
       <c r="C17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
@@ -4842,13 +4840,13 @@
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>132</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -4876,24 +4874,24 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" s="20" t="s">
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
ITSADSSD-19693 - EoM - 'Checklist Management 2' due date
Change project version, email address in config and retry for Item and Due date field
</commit_message>
<xml_diff>
--- a/Processes/UQGS_EOM_proc_SInetDueDateUpdate_1.0/Data/Config.xlsx
+++ b/Processes/UQGS_EOM_proc_SInetDueDateUpdate_1.0/Data/Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uqsjose6\workspaces\FORK\RpaUiPathProcess\Processes\UQGS_EOM_proc_SInetDueDateUpdate_1.0\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uqmgupt1\Documents\UiPath\RpaUiPathProcess\Processes\UQGS_EOM_proc_SInetDueDateUpdate_1.0\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -487,7 +487,7 @@
     <t>List of allowed Item codes</t>
   </si>
   <si>
-    <t>bpm.ads@its.uq.edu.au</t>
+    <t xml:space="preserve">rpa.ads@its.uq.edu.au </t>
   </si>
 </sst>
 </file>
@@ -1143,7 +1143,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -2447,6 +2449,10 @@
     <row r="999" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="11" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B19" r:id="rId1"/>
+    <hyperlink ref="B20:B22" r:id="rId2" display="rpa.ads@its.uq.edu.au "/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">

</xml_diff>